<commit_message>
Changed Capacitor in BOM
Bigger!
</commit_message>
<xml_diff>
--- a/RenardESPBOM.xlsx
+++ b/RenardESPBOM.xlsx
@@ -63,9 +63,6 @@
     <t>Capacitor Pol</t>
   </si>
   <si>
-    <t>P15787CT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capacitor  </t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1189-2375-ND</t>
   </si>
 </sst>
 </file>
@@ -480,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -552,13 +552,20 @@
         <v>27</v>
       </c>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="K2">
+        <f>J2*D2</f>
+        <v>0.41599999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -567,27 +574,34 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.35</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F20" si="0">E3*D3</f>
-        <v>0.35</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G3">
-        <v>0.11443</v>
+        <v>0.11008</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H21" si="1">G3*100*D3</f>
-        <v>11.443</v>
+        <v>11.007999999999999</v>
       </c>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>0.156</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K11" si="2">J3*D3</f>
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -610,13 +624,20 @@
         <v>12.09</v>
       </c>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -638,13 +659,20 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -666,13 +694,20 @@
         <f t="shared" si="1"/>
         <v>113.99999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>1.488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -694,13 +729,20 @@
         <f t="shared" si="1"/>
         <v>56.999999999999993</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0.749</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -722,13 +764,20 @@
         <f t="shared" si="1"/>
         <v>2.19</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -750,13 +799,20 @@
         <f t="shared" si="1"/>
         <v>44.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>9.61</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>0.48049999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -778,13 +834,20 @@
         <f t="shared" si="1"/>
         <v>56.760000000000005</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>2.34</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0.7722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -806,8 +869,15 @@
         <f t="shared" si="1"/>
         <v>6.7199999999999989</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -817,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -828,13 +898,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>0.1</v>
@@ -852,8 +922,14 @@
       <c r="H14">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>1.3</v>
+      </c>
+      <c r="K14">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -863,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -873,12 +949,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -897,8 +973,11 @@
         <f t="shared" si="1"/>
         <v>556</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -908,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -918,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -928,32 +1007,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>14.8</v>
+      </c>
+      <c r="K24">
+        <f>J24/4</f>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>15.3</v>
+      </c>
+      <c r="K25">
+        <f>J25/4</f>
+        <v>3.8250000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>9</v>
       </c>
       <c r="F28">
         <f>SUM(F2:F25)</f>
-        <v>13.272699999999999</v>
+        <v>13.212699999999998</v>
       </c>
       <c r="H28">
         <f>SUM(H2:H25)</f>
-        <v>1087.8029999999999</v>
+        <v>1087.3679999999999</v>
       </c>
       <c r="J28">
         <f>H28/100</f>
-        <v>10.878029999999999</v>
+        <v>10.87368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RevE with 8 pin DIP adapter
Trade the break away PCB adapter for a COTS ribbon cable DIP adapter.
</commit_message>
<xml_diff>
--- a/RenardESPBOM.xlsx
+++ b/RenardESPBOM.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Description</t>
   </si>
@@ -69,18 +70,6 @@
     <t>399-9776-ND</t>
   </si>
   <si>
-    <t>6 pin connector</t>
-  </si>
-  <si>
-    <t>609-2845-ND</t>
-  </si>
-  <si>
-    <t>6 pin csocket</t>
-  </si>
-  <si>
-    <t>609-2841-ND</t>
-  </si>
-  <si>
     <t>8 pin socket</t>
   </si>
   <si>
@@ -124,6 +113,24 @@
   </si>
   <si>
     <t>1189-2375-ND</t>
+  </si>
+  <si>
+    <t>8 pin Shourded socket</t>
+  </si>
+  <si>
+    <t>8 pin connector</t>
+  </si>
+  <si>
+    <t>609-3530-ND </t>
+  </si>
+  <si>
+    <t>609-3568-ND </t>
+  </si>
+  <si>
+    <t>DIP adapter</t>
+  </si>
+  <si>
+    <t>5746613-1-ND</t>
   </si>
 </sst>
 </file>
@@ -480,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +572,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -577,14 +584,14 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F20" si="0">E3*D3</f>
+        <f t="shared" ref="F3:F21" si="0">E3*D3</f>
         <v>0.28999999999999998</v>
       </c>
       <c r="G3">
         <v>0.11008</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H21" si="1">G3*100*D3</f>
+        <f t="shared" ref="H3:H22" si="1">G3*100*D3</f>
         <v>11.007999999999999</v>
       </c>
       <c r="I3" s="1"/>
@@ -592,7 +599,7 @@
         <v>0.156</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K11" si="2">J3*D3</f>
+        <f t="shared" ref="K3:K12" si="2">J3*D3</f>
         <v>0.156</v>
       </c>
     </row>
@@ -634,80 +641,80 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.71</v>
+        <v>0.8</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>1.42</v>
+        <v>0.8</v>
       </c>
       <c r="G5">
-        <v>0.5</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>57.199999999999996</v>
       </c>
       <c r="J5">
         <v>0.59499999999999997</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>1.19</v>
+        <v>0.59499999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0.79</v>
+        <v>0.94</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>1.58</v>
+        <v>0.94</v>
       </c>
       <c r="G6">
-        <v>0.56999999999999995</v>
+        <v>0.71</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>113.99999999999999</v>
+        <v>71</v>
       </c>
       <c r="J6">
         <v>0.74399999999999999</v>
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>1.488</v>
+        <v>0.74399999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -739,10 +746,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -751,144 +758,161 @@
         <v>1</v>
       </c>
       <c r="E8">
+        <v>2.38</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2.38</v>
+      </c>
+      <c r="G8">
+        <v>1.89</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>0.1</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>2.1899999999999999E-2</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <f t="shared" si="1"/>
         <v>2.19</v>
       </c>
-      <c r="J8">
+      <c r="J9">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="K8">
+      <c r="K9">
         <f t="shared" si="2"/>
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>0.05</v>
-      </c>
-      <c r="E9">
-        <v>9.61</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0.48049999999999998</v>
-      </c>
-      <c r="G9">
-        <v>8.92</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>44.6</v>
-      </c>
-      <c r="J9">
-        <v>9.61</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="2"/>
-        <v>0.48049999999999998</v>
-      </c>
-    </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10">
-        <v>0.33</v>
+        <v>0.11</v>
       </c>
       <c r="E10">
-        <v>2.34</v>
+        <v>9.61</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0.7722</v>
+        <v>1.0570999999999999</v>
       </c>
       <c r="G10">
-        <v>1.72</v>
+        <v>8.92</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>56.760000000000005</v>
+        <v>98.12</v>
       </c>
       <c r="J10">
-        <v>2.34</v>
+        <v>9.61</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>0.7722</v>
+        <v>1.0570999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>0.33</v>
       </c>
       <c r="E11">
-        <v>0.1</v>
+        <v>2.34</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.7722</v>
       </c>
       <c r="G11">
-        <v>2.24E-2</v>
+        <v>1.72</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>6.7199999999999989</v>
+        <v>56.760000000000005</v>
       </c>
       <c r="J11">
-        <v>5.1999999999999998E-2</v>
+        <v>2.34</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
+        <v>0.7722</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G12">
+        <v>2.24E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>6.7199999999999989</v>
+      </c>
+      <c r="J12">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
         <v>0.156</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -899,44 +923,45 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" s="2"/>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14">
+      <c r="B15" s="2"/>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
         <v>0.1</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>10</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>100</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>100</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <v>1.3</v>
       </c>
-      <c r="K14">
+      <c r="K15">
         <v>1.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -950,41 +975,41 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
         <v>1</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>5.56</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <f t="shared" si="0"/>
         <v>5.56</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>5.56</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <f t="shared" si="1"/>
         <v>556</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>5.56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1008,54 +1033,64 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>34</v>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J24">
-        <v>14.8</v>
-      </c>
-      <c r="K24">
-        <f>J24/4</f>
-        <v>3.7</v>
+      <c r="D24" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J25">
-        <v>15.3</v>
+        <v>14.8</v>
       </c>
       <c r="K25">
         <f>J25/4</f>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>15.3</v>
+      </c>
+      <c r="K26">
+        <f>J26/4</f>
         <v>3.8250000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
         <v>9</v>
       </c>
-      <c r="F28">
-        <f>SUM(F2:F25)</f>
-        <v>13.212699999999998</v>
-      </c>
-      <c r="H28">
-        <f>SUM(H2:H25)</f>
-        <v>1087.3679999999999</v>
-      </c>
-      <c r="J28">
-        <f>H28/100</f>
-        <v>10.87368</v>
+      <c r="F29">
+        <f>SUM(F2:F26)</f>
+        <v>14.909300000000002</v>
+      </c>
+      <c r="H29">
+        <f>SUM(H2:H26)</f>
+        <v>1244.088</v>
+      </c>
+      <c r="J29">
+        <f>H29/100</f>
+        <v>12.44088</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>